<commit_message>
integrate the excel generation in teacher console
</commit_message>
<xml_diff>
--- a/Child_Teacher/core/B.xlsx
+++ b/Child_Teacher/core/B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Names</t>
   </si>
@@ -34,31 +34,37 @@
     <t>Paco</t>
   </si>
   <si>
-    <t>Pel otro</t>
+    <t>Lola</t>
+  </si>
+  <si>
+    <t>Javi</t>
+  </si>
+  <si>
+    <t>galdiolo</t>
+  </si>
+  <si>
+    <t>flor</t>
+  </si>
+  <si>
+    <t>bloso</t>
+  </si>
+  <si>
+    <t>palmera</t>
   </si>
   <si>
     <t>Paco:</t>
   </si>
   <si>
-    <t>galdiolo</t>
-  </si>
-  <si>
-    <t>flor</t>
-  </si>
-  <si>
-    <t>palmera</t>
-  </si>
-  <si>
-    <t>bloso</t>
+    <t>1</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Pel otro:</t>
+    <t>Lola:</t>
+  </si>
+  <si>
+    <t>Javi:</t>
   </si>
 </sst>
 </file>
@@ -140,29 +146,35 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Paco</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Pel otro</c:v>
+                  <c:v>Lola</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Javi</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$26</c:f>
+              <c:f>Sheet1!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -176,15 +188,18 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$26</c:f>
+              <c:f>Sheet1!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -279,13 +294,24 @@
             <c:v>Fallos por palabra</c:v>
           </c:tx>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="4"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>galdiolo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>flor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>bloso</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>palmera</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -293,6 +319,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -306,7 +344,6 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
@@ -398,10 +435,10 @@
                   <c:v>flor</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>bloso</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>palmera</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>bloso</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -413,10 +450,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -498,7 +535,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Pel otro</a:t>
+              <a:t>Lola</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -525,13 +562,13 @@
                   <c:v>galdiolo</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>bloso</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>flor</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>palmera</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>bloso</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -543,7 +580,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -552,7 +589,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -584,6 +621,136 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50040001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFC2"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Javi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Fallos por palabra</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$12:$K$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>flor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>palmera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>galdiolo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bloso</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$12:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50050001"/>
+        <c:axId val="50050002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50050001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50050002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -730,6 +897,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1023,7 +1220,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L10"/>
+  <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1060,19 +1257,25 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -1080,19 +1283,40 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>20</v>
       </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
       <c r="K3" t="s">
         <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:12">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
@@ -1101,27 +1325,33 @@
       </c>
     </row>
     <row r="5" spans="2:12">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
       <c r="K5" t="s">
         <v>11</v>
       </c>
       <c r="L5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:12">
       <c r="J7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
       </c>
       <c r="L7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:12">
       <c r="K8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L8" t="s">
         <v>13</v>
@@ -1129,10 +1359,10 @@
     </row>
     <row r="9" spans="2:12">
       <c r="K9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -1140,7 +1370,42 @@
         <v>11</v>
       </c>
       <c r="L10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="K14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement cv2 on the game
</commit_message>
<xml_diff>
--- a/Child_Teacher/core/B.xlsx
+++ b/Child_Teacher/core/B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Names</t>
   </si>
@@ -31,40 +31,28 @@
     <t>Fails</t>
   </si>
   <si>
-    <t>Paco</t>
-  </si>
-  <si>
-    <t>Lola</t>
-  </si>
-  <si>
-    <t>Javi</t>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>flor</t>
+  </si>
+  <si>
+    <t>bloso</t>
+  </si>
+  <si>
+    <t>palmera</t>
   </si>
   <si>
     <t>galdiolo</t>
   </si>
   <si>
-    <t>flor</t>
-  </si>
-  <si>
-    <t>bloso</t>
-  </si>
-  <si>
-    <t>palmera</t>
-  </si>
-  <si>
-    <t>Paco:</t>
+    <t>Luis:</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Lola:</t>
-  </si>
-  <si>
-    <t>Javi:</t>
   </si>
 </sst>
 </file>
@@ -146,35 +134,23 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>Sheet1!$B$2:$B$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Paco</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lola</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Javi</c:v>
+                  <c:v>Luis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:f>Sheet1!$C$2:$C$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -188,18 +164,12 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:f>Sheet1!$D$2:$D$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,16 +269,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>flor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bloso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>palmera</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>galdiolo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>flor</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>bloso</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>palmera</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -405,7 +375,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Paco</a:t>
+              <a:t>Luis</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -429,16 +399,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>flor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bloso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>palmera</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>galdiolo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>flor</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>bloso</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>palmera</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -450,7 +420,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -459,7 +429,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,266 +461,6 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFC2"/>
-        </a:solidFill>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Lola</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Fallos por palabra</c:v>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$K$7:$K$10</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>galdiolo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>bloso</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>flor</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>palmera</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$L$7:$L$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50040001"/>
-        <c:axId val="50040002"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="50040001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50040002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50040002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50040001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFC2"/>
-        </a:solidFill>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Javi</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Fallos por palabra</c:v>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$K$12:$K$15</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>flor</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>palmera</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>galdiolo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>bloso</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$L$12:$L$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50050001"/>
-        <c:axId val="50050002"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="50050001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50050002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50050002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50050001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -867,66 +577,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1220,7 +870,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1257,155 +907,67 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:12">
       <c r="G5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12">
-      <c r="K8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12">
-      <c r="K9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12">
-      <c r="K10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12">
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12">
-      <c r="K13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12">
-      <c r="K14" t="s">
-        <v>8</v>
-      </c>
-      <c r="L14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12">
-      <c r="K15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create the 4, 8 and 12 version
</commit_message>
<xml_diff>
--- a/Child_Teacher/core/B.xlsx
+++ b/Child_Teacher/core/B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Names</t>
   </si>
@@ -31,22 +31,46 @@
     <t>Fails</t>
   </si>
   <si>
-    <t>Luis</t>
+    <t>Paco</t>
+  </si>
+  <si>
+    <t>falda</t>
+  </si>
+  <si>
+    <t>aporbar</t>
+  </si>
+  <si>
+    <t>abarzar</t>
+  </si>
+  <si>
+    <t>plamera</t>
+  </si>
+  <si>
+    <t>furta</t>
+  </si>
+  <si>
+    <t>tornillo</t>
+  </si>
+  <si>
+    <t>galdiolo</t>
+  </si>
+  <si>
+    <t>palmera</t>
+  </si>
+  <si>
+    <t>parque</t>
+  </si>
+  <si>
+    <t>tractor</t>
   </si>
   <si>
     <t>flor</t>
   </si>
   <si>
-    <t>bloso</t>
-  </si>
-  <si>
-    <t>palmera</t>
-  </si>
-  <si>
-    <t>galdiolo</t>
-  </si>
-  <si>
-    <t>Luis:</t>
+    <t>adrono</t>
+  </si>
+  <si>
+    <t>Paco:</t>
   </si>
   <si>
     <t>0</t>
@@ -138,7 +162,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Luis</c:v>
+                  <c:v>Paco</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -150,7 +174,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -169,7 +193,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -269,16 +293,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>flor</c:v>
+                  <c:v>falda</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bloso</c:v>
+                  <c:v>aporbar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>palmera</c:v>
+                  <c:v>abarzar</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>galdiolo</c:v>
+                  <c:v>plamera</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -375,7 +399,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Luis</a:t>
+              <a:t>Paco</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -399,16 +423,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>flor</c:v>
+                  <c:v>falda</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bloso</c:v>
+                  <c:v>aporbar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>palmera</c:v>
+                  <c:v>abarzar</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>galdiolo</c:v>
+                  <c:v>plamera</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -870,7 +894,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L5"/>
+  <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -907,10 +931,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -919,13 +943,13 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -939,7 +963,7 @@
         <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:12">
@@ -953,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -967,7 +991,119 @@
         <v>9</v>
       </c>
       <c r="L5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="G8" t="s">
         <v>12</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>